<commit_message>
Replaced PageFactory with By locators in Page Object classes
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="8856" windowHeight="4956"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="8556" windowHeight="4656"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -576,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>